<commit_message>
Add cards.xlsx and update Board component to read it
</commit_message>
<xml_diff>
--- a/public/cards.xlsx
+++ b/public/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matyashirman/fair-quest/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5B2123-6A52-7448-8FAC-88156CFE049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D9B3FD-B93E-5A43-87CC-14C308BEDE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15820" xr2:uid="{5302F086-E48E-5A49-940A-984B7827E756}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>